<commit_message>
added max block adj types
</commit_message>
<xml_diff>
--- a/Projects/DELMONTEUS/Data/DelMonte_KPI Template v0.4.xlsx
+++ b/Projects/DELMONTEUS/Data/DelMonte_KPI Template v0.4.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="8"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="KPIs" sheetId="1" state="visible" r:id="rId2"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="985" uniqueCount="196">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="984" uniqueCount="196">
   <si>
     <t xml:space="preserve">KPI Name</t>
   </si>
@@ -541,6 +541,9 @@
     <t xml:space="preserve">GREEN GIANT</t>
   </si>
   <si>
+    <t xml:space="preserve">MULTIPACK,MULTIPK</t>
+  </si>
+  <si>
     <t xml:space="preserve">Orientation</t>
   </si>
   <si>
@@ -565,7 +568,7 @@
     <t xml:space="preserve">CORE</t>
   </si>
   <si>
-    <t xml:space="preserve">top, bottom</t>
+    <t xml:space="preserve">top,bottom,left,right</t>
   </si>
   <si>
     <t xml:space="preserve">AFC</t>
@@ -599,9 +602,6 @@
   </si>
   <si>
     <t xml:space="preserve">CRANBERRY</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Inverse</t>
   </si>
   <si>
     <t xml:space="preserve">SGL-SRV, MLTI-SRV</t>
@@ -2269,7 +2269,7 @@
       <c r="D3" s="10"/>
       <c r="E3" s="10"/>
       <c r="F3" s="10" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="105" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2301,7 +2301,7 @@
       <c r="D5" s="10"/>
       <c r="E5" s="10"/>
       <c r="F5" s="10" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="90" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2317,7 +2317,7 @@
       <c r="D6" s="10"/>
       <c r="E6" s="10"/>
       <c r="F6" s="10" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="90" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2333,7 +2333,7 @@
       <c r="D7" s="10"/>
       <c r="E7" s="10"/>
       <c r="F7" s="10" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="90" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2349,7 +2349,7 @@
       <c r="D8" s="10"/>
       <c r="E8" s="10"/>
       <c r="F8" s="10" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="90" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2369,7 +2369,7 @@
         <v>162</v>
       </c>
       <c r="F9" s="10" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="90" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2389,7 +2389,7 @@
         <v>162</v>
       </c>
       <c r="F10" s="10" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="105" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2409,7 +2409,7 @@
         <v>162</v>
       </c>
       <c r="F11" s="10" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="90" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2429,7 +2429,7 @@
         <v>163</v>
       </c>
       <c r="F12" s="10" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="90" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2449,7 +2449,7 @@
         <v>163</v>
       </c>
       <c r="F13" s="10" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="105" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2469,7 +2469,7 @@
         <v>163</v>
       </c>
       <c r="F14" s="10" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2480,12 +2480,12 @@
         <v>119</v>
       </c>
       <c r="C15" s="10" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="D15" s="9"/>
       <c r="E15" s="9"/>
       <c r="F15" s="10" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2496,12 +2496,12 @@
         <v>119</v>
       </c>
       <c r="C16" s="10" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="D16" s="9"/>
       <c r="E16" s="9"/>
       <c r="F16" s="10" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="90" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2512,12 +2512,12 @@
         <v>119</v>
       </c>
       <c r="C17" s="10" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="D17" s="9"/>
       <c r="E17" s="9"/>
       <c r="F17" s="10" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="90" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2577,7 +2577,7 @@
         <v>130</v>
       </c>
       <c r="F20" s="10" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="105" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2637,7 +2637,7 @@
         <v>132</v>
       </c>
       <c r="F23" s="10" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="90" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2657,7 +2657,7 @@
         <v>130</v>
       </c>
       <c r="F24" s="10" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="105" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2677,7 +2677,7 @@
         <v>130</v>
       </c>
       <c r="F25" s="10" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="105" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2697,7 +2697,7 @@
         <v>130</v>
       </c>
       <c r="F26" s="10" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="105" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2717,7 +2717,7 @@
         <v>130</v>
       </c>
       <c r="F27" s="10" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="105" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2737,7 +2737,7 @@
         <v>132</v>
       </c>
       <c r="F28" s="10" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="120" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2757,7 +2757,7 @@
         <v>132</v>
       </c>
       <c r="F29" s="10" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="120" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2777,7 +2777,7 @@
         <v>132</v>
       </c>
       <c r="F30" s="10" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="120" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2797,7 +2797,7 @@
         <v>132</v>
       </c>
       <c r="F31" s="10" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2811,13 +2811,13 @@
         <v>142</v>
       </c>
       <c r="D32" s="9" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="E32" s="9" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="F32" s="10" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2831,13 +2831,13 @@
         <v>142</v>
       </c>
       <c r="D33" s="9" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="E33" s="9" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="F33" s="10" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="90" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2851,13 +2851,13 @@
         <v>142</v>
       </c>
       <c r="D34" s="9" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="E34" s="9" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="F34" s="10" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
     </row>
   </sheetData>
@@ -3036,19 +3036,19 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="1:65536"/>
+  <dimension ref="A1:AMI2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="11.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="34.2925925925926"/>
     <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="8.62222222222222"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -3058,17 +3058,14 @@
       <c r="C1" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="D1" s="5" t="s">
-        <v>188</v>
-      </c>
+      <c r="AMD1" s="20"/>
       <c r="AME1" s="20"/>
       <c r="AMF1" s="20"/>
       <c r="AMG1" s="20"/>
       <c r="AMH1" s="20"/>
       <c r="AMI1" s="20"/>
-      <c r="AMJ1" s="20"/>
-    </row>
-    <row r="2" customFormat="false" ht="105" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="2" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="9" t="s">
         <v>66</v>
       </c>
@@ -3078,12 +3075,8 @@
       <c r="C2" s="10" t="s">
         <v>189</v>
       </c>
-      <c r="D2" s="9" t="n">
-        <v>1</v>
-      </c>
-      <c r="E2" s="21"/>
-    </row>
-    <row r="1048576" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+      <c r="D2" s="21"/>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -3123,10 +3116,10 @@
         <v>122</v>
       </c>
       <c r="D1" s="13" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="E1" s="13" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="F1" s="13" t="s">
         <v>123</v>
@@ -3135,10 +3128,10 @@
         <v>124</v>
       </c>
       <c r="H1" s="13" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="I1" s="13" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="J1" s="22" t="s">
         <v>53</v>
@@ -3167,7 +3160,7 @@
         <v>117</v>
       </c>
       <c r="G2" s="23" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="H2" s="23" t="s">
         <v>141</v>
@@ -3202,7 +3195,7 @@
         <v>117</v>
       </c>
       <c r="G3" s="23" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="H3" s="23" t="s">
         <v>141</v>
@@ -3237,7 +3230,7 @@
         <v>117</v>
       </c>
       <c r="G4" s="23" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="H4" s="23" t="s">
         <v>141</v>
@@ -3268,7 +3261,7 @@
         <v>117</v>
       </c>
       <c r="G5" s="23" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="H5" s="14"/>
       <c r="I5" s="14"/>
@@ -3453,7 +3446,7 @@
         <v>7</v>
       </c>
       <c r="H3" s="10" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="105" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3553,7 +3546,7 @@
         <v>131</v>
       </c>
       <c r="H7" s="10" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="105" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3631,7 +3624,7 @@
         <v>131</v>
       </c>
       <c r="H10" s="10" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
     </row>
   </sheetData>
@@ -4234,8 +4227,8 @@
   </sheetPr>
   <dimension ref="A1:E65536"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C11" activeCellId="0" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25"/>
@@ -4402,7 +4395,7 @@
       <c r="D10" s="10"/>
       <c r="E10" s="10"/>
     </row>
-    <row r="11" customFormat="false" ht="90" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="14" t="s">
         <v>28</v>
       </c>
@@ -4410,7 +4403,7 @@
         <v>155</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>156</v>
+        <v>168</v>
       </c>
       <c r="D11" s="10"/>
       <c r="E11" s="10"/>
@@ -4449,8 +4442,8 @@
   </sheetPr>
   <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F4" activeCellId="0" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25"/>
@@ -4469,7 +4462,7 @@
         <v>116</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="90" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4483,7 +4476,7 @@
         <v>142</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="105" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4497,7 +4490,7 @@
         <v>142</v>
       </c>
       <c r="D3" s="10" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="105" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4511,7 +4504,7 @@
         <v>167</v>
       </c>
       <c r="D4" s="10" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="120" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4525,7 +4518,7 @@
         <v>167</v>
       </c>
       <c r="D5" s="10" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="105" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4539,7 +4532,7 @@
         <v>130</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="105" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4553,7 +4546,7 @@
         <v>130</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="120" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4567,7 +4560,7 @@
         <v>132</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="120" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4581,7 +4574,7 @@
         <v>132</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
     </row>
   </sheetData>
@@ -4603,13 +4596,16 @@
   <dimension ref="A1:J5"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="46.9962962962963"/>
-    <col collapsed="false" hidden="false" max="9" min="2" style="0" width="11.8962962962963"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="59.1037037037037"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.7259259259259"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="11.8962962962963"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15.2296296296296"/>
+    <col collapsed="false" hidden="false" max="9" min="5" style="0" width="11.8962962962963"/>
     <col collapsed="false" hidden="false" max="10" min="10" style="0" width="11.5962962962963"/>
     <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="8.62222222222222"/>
   </cols>
@@ -4625,10 +4621,10 @@
         <v>122</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="F1" s="5" t="s">
         <v>123</v>
@@ -4637,16 +4633,16 @@
         <v>124</v>
       </c>
       <c r="H1" s="5" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="I1" s="5" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="J1" s="5" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="120" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="9" t="s">
         <v>21</v>
       </c>
@@ -4666,7 +4662,7 @@
         <v>117</v>
       </c>
       <c r="G2" s="10" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="H2" s="10" t="s">
         <v>141</v>
@@ -4675,10 +4671,10 @@
         <v>142</v>
       </c>
       <c r="J2" s="10" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="90" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="9" t="s">
         <v>23</v>
       </c>
@@ -4694,15 +4690,15 @@
         <v>117</v>
       </c>
       <c r="G3" s="10" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="H3" s="10"/>
       <c r="I3" s="10"/>
       <c r="J3" s="10" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="90" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="9" t="s">
         <v>78</v>
       </c>
@@ -4713,10 +4709,10 @@
         <v>142</v>
       </c>
       <c r="D4" s="10" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="E4" s="10" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="F4" s="9" t="s">
         <v>130</v>
@@ -4727,10 +4723,10 @@
       <c r="H4" s="9"/>
       <c r="I4" s="9"/>
       <c r="J4" s="10" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="9" t="s">
         <v>90</v>
       </c>
@@ -4755,7 +4751,7 @@
       <c r="H5" s="10"/>
       <c r="I5" s="3"/>
       <c r="J5" s="10" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
     </row>
   </sheetData>
@@ -4777,7 +4773,7 @@
   <dimension ref="A1:K5"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G5" activeCellId="0" sqref="G5"/>
+      <selection pane="topLeft" activeCell="C40" activeCellId="0" sqref="C40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4806,10 +4802,10 @@
         <v>122</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="F1" s="5" t="s">
         <v>123</v>
@@ -4818,13 +4814,13 @@
         <v>124</v>
       </c>
       <c r="H1" s="5" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="I1" s="5" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="J1" s="5" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="K1" s="5" t="s">
         <v>139</v>
@@ -4838,7 +4834,7 @@
         <v>155</v>
       </c>
       <c r="C2" s="15" t="s">
-        <v>156</v>
+        <v>168</v>
       </c>
       <c r="D2" s="16"/>
       <c r="E2" s="15"/>
@@ -4846,15 +4842,15 @@
         <v>157</v>
       </c>
       <c r="G2" s="17" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="H2" s="17"/>
       <c r="I2" s="17"/>
       <c r="J2" s="17" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="K2" s="17" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4873,15 +4869,15 @@
         <v>157</v>
       </c>
       <c r="G3" s="17" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="H3" s="17"/>
       <c r="I3" s="17"/>
       <c r="J3" s="17" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="K3" s="17" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4892,7 +4888,7 @@
         <v>155</v>
       </c>
       <c r="C4" s="15" t="s">
-        <v>156</v>
+        <v>168</v>
       </c>
       <c r="D4" s="16" t="s">
         <v>141</v>
@@ -4904,7 +4900,7 @@
         <v>157</v>
       </c>
       <c r="G4" s="17" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="H4" s="18" t="s">
         <v>141</v>
@@ -4913,10 +4909,10 @@
         <v>142</v>
       </c>
       <c r="J4" s="18" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="K4" s="17" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4939,7 +4935,7 @@
         <v>157</v>
       </c>
       <c r="G5" s="17" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="H5" s="17" t="s">
         <v>141</v>
@@ -4948,10 +4944,10 @@
         <v>142</v>
       </c>
       <c r="J5" s="17" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="K5" s="17" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
     </row>
   </sheetData>
@@ -4972,7 +4968,7 @@
   </sheetPr>
   <dimension ref="A1:J3"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="G9" activeCellId="0" sqref="G9"/>
     </sheetView>
   </sheetViews>
@@ -4994,10 +4990,10 @@
         <v>122</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="F1" s="5" t="s">
         <v>123</v>
@@ -5006,10 +5002,10 @@
         <v>124</v>
       </c>
       <c r="H1" s="5" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="I1" s="5" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="J1" s="5" t="s">
         <v>139</v>
@@ -5026,10 +5022,10 @@
         <v>142</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="F2" s="9" t="s">
         <v>128</v>
@@ -5040,7 +5036,7 @@
       <c r="H2" s="9"/>
       <c r="I2" s="9"/>
       <c r="J2" s="10" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5054,10 +5050,10 @@
         <v>142</v>
       </c>
       <c r="D3" s="10" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="E3" s="10" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="F3" s="10" t="s">
         <v>141</v>
@@ -5072,7 +5068,7 @@
         <v>130</v>
       </c>
       <c r="J3" s="10" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated shelf region shelf placement serial adj block together
</commit_message>
<xml_diff>
--- a/Projects/DELMONTEUS/Data/DelMonte_KPI Template v0.4.xlsx
+++ b/Projects/DELMONTEUS/Data/DelMonte_KPI Template v0.4.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="5"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="KPIs" sheetId="1" state="visible" r:id="rId2"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="984" uniqueCount="196">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="990" uniqueCount="198">
   <si>
     <t xml:space="preserve">KPI Name</t>
   </si>
@@ -505,7 +505,7 @@
     <t xml:space="preserve">MULTIPK</t>
   </si>
   <si>
-    <t xml:space="preserve">MULTIPACK</t>
+    <t xml:space="preserve">MULTIPACK,MULTIPK</t>
   </si>
   <si>
     <t xml:space="preserve">DLM_ VEGSZ(C)</t>
@@ -541,9 +541,6 @@
     <t xml:space="preserve">GREEN GIANT</t>
   </si>
   <si>
-    <t xml:space="preserve">MULTIPACK,MULTIPK</t>
-  </si>
-  <si>
     <t xml:space="preserve">Orientation</t>
   </si>
   <si>
@@ -574,6 +571,12 @@
     <t xml:space="preserve">AFC</t>
   </si>
   <si>
+    <t xml:space="preserve">A Param 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A Value 3</t>
+  </si>
+  <si>
     <t xml:space="preserve">Unit</t>
   </si>
   <si>
@@ -581,6 +584,9 @@
   </si>
   <si>
     <t xml:space="preserve">VEG_TYPE(C)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">left,right,top,bottom</t>
   </si>
   <si>
     <t xml:space="preserve">left,right</t>
@@ -634,7 +640,7 @@
     <numFmt numFmtId="165" formatCode="0%"/>
     <numFmt numFmtId="166" formatCode="@"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="8">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -684,13 +690,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="5">
@@ -760,7 +759,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="25">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -847,10 +846,6 @@
     </xf>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -950,8 +945,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="45.7888888888889"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="8.62222222222222"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="49.2925925925926"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="9.21111111111111"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2217,7 +2212,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.62222222222222"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="9.21111111111111"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2269,7 +2264,7 @@
       <c r="D3" s="10"/>
       <c r="E3" s="10"/>
       <c r="F3" s="10" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="105" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2301,7 +2296,7 @@
       <c r="D5" s="10"/>
       <c r="E5" s="10"/>
       <c r="F5" s="10" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="90" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2317,7 +2312,7 @@
       <c r="D6" s="10"/>
       <c r="E6" s="10"/>
       <c r="F6" s="10" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="90" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2333,7 +2328,7 @@
       <c r="D7" s="10"/>
       <c r="E7" s="10"/>
       <c r="F7" s="10" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="90" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2349,7 +2344,7 @@
       <c r="D8" s="10"/>
       <c r="E8" s="10"/>
       <c r="F8" s="10" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="90" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2369,7 +2364,7 @@
         <v>162</v>
       </c>
       <c r="F9" s="10" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="90" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2389,7 +2384,7 @@
         <v>162</v>
       </c>
       <c r="F10" s="10" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="105" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2409,7 +2404,7 @@
         <v>162</v>
       </c>
       <c r="F11" s="10" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="90" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2429,7 +2424,7 @@
         <v>163</v>
       </c>
       <c r="F12" s="10" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="90" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2449,7 +2444,7 @@
         <v>163</v>
       </c>
       <c r="F13" s="10" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="105" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2469,7 +2464,7 @@
         <v>163</v>
       </c>
       <c r="F14" s="10" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2480,12 +2475,12 @@
         <v>119</v>
       </c>
       <c r="C15" s="10" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="D15" s="9"/>
       <c r="E15" s="9"/>
       <c r="F15" s="10" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2496,12 +2491,12 @@
         <v>119</v>
       </c>
       <c r="C16" s="10" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="D16" s="9"/>
       <c r="E16" s="9"/>
       <c r="F16" s="10" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="90" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2512,12 +2507,12 @@
         <v>119</v>
       </c>
       <c r="C17" s="10" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="D17" s="9"/>
       <c r="E17" s="9"/>
       <c r="F17" s="10" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="90" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2577,7 +2572,7 @@
         <v>130</v>
       </c>
       <c r="F20" s="10" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="105" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2637,7 +2632,7 @@
         <v>132</v>
       </c>
       <c r="F23" s="10" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="90" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2657,7 +2652,7 @@
         <v>130</v>
       </c>
       <c r="F24" s="10" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="105" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2677,7 +2672,7 @@
         <v>130</v>
       </c>
       <c r="F25" s="10" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="105" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2697,7 +2692,7 @@
         <v>130</v>
       </c>
       <c r="F26" s="10" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="105" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2717,7 +2712,7 @@
         <v>130</v>
       </c>
       <c r="F27" s="10" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="105" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2737,7 +2732,7 @@
         <v>132</v>
       </c>
       <c r="F28" s="10" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="120" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2757,7 +2752,7 @@
         <v>132</v>
       </c>
       <c r="F29" s="10" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="120" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2777,7 +2772,7 @@
         <v>132</v>
       </c>
       <c r="F30" s="10" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="120" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2797,7 +2792,7 @@
         <v>132</v>
       </c>
       <c r="F31" s="10" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2811,13 +2806,13 @@
         <v>142</v>
       </c>
       <c r="D32" s="9" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E32" s="9" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F32" s="10" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2831,13 +2826,13 @@
         <v>142</v>
       </c>
       <c r="D33" s="9" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E33" s="9" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F33" s="10" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="90" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2851,13 +2846,13 @@
         <v>142</v>
       </c>
       <c r="D34" s="9" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E34" s="9" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F34" s="10" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
     </row>
   </sheetData>
@@ -2884,7 +2879,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.62222222222222"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="9.21111111111111"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3044,8 +3039,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="34.2925925925926"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="8.62222222222222"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="36.9444444444444"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="9.21111111111111"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3073,7 +3068,7 @@
         <v>161</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="D2" s="21"/>
     </row>
@@ -3101,8 +3096,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="65.5592592592593"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="8.62222222222222"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="70.6518518518518"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="9.21111111111111"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3116,10 +3111,10 @@
         <v>122</v>
       </c>
       <c r="D1" s="13" t="s">
+        <v>171</v>
+      </c>
+      <c r="E1" s="13" t="s">
         <v>172</v>
-      </c>
-      <c r="E1" s="13" t="s">
-        <v>173</v>
       </c>
       <c r="F1" s="13" t="s">
         <v>123</v>
@@ -3128,12 +3123,12 @@
         <v>124</v>
       </c>
       <c r="H1" s="13" t="s">
+        <v>173</v>
+      </c>
+      <c r="I1" s="13" t="s">
         <v>174</v>
       </c>
-      <c r="I1" s="13" t="s">
-        <v>175</v>
-      </c>
-      <c r="J1" s="22" t="s">
+      <c r="J1" s="5" t="s">
         <v>53</v>
       </c>
       <c r="K1" s="13" t="s">
@@ -3144,132 +3139,132 @@
       <c r="A2" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="B2" s="23" t="s">
+      <c r="B2" s="22" t="s">
         <v>117</v>
       </c>
-      <c r="C2" s="23" t="s">
+      <c r="C2" s="22" t="s">
         <v>165</v>
       </c>
-      <c r="D2" s="23" t="s">
+      <c r="D2" s="22" t="s">
         <v>141</v>
       </c>
       <c r="E2" s="14" t="s">
         <v>142</v>
       </c>
-      <c r="F2" s="23" t="s">
+      <c r="F2" s="22" t="s">
         <v>117</v>
       </c>
-      <c r="G2" s="23" t="s">
-        <v>176</v>
-      </c>
-      <c r="H2" s="23" t="s">
+      <c r="G2" s="22" t="s">
+        <v>175</v>
+      </c>
+      <c r="H2" s="22" t="s">
         <v>141</v>
       </c>
       <c r="I2" s="14" t="s">
         <v>142</v>
       </c>
       <c r="J2" s="14" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="K2" s="0" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="136.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="B3" s="23" t="s">
+      <c r="B3" s="22" t="s">
         <v>117</v>
       </c>
-      <c r="C3" s="23" t="s">
+      <c r="C3" s="22" t="s">
         <v>165</v>
       </c>
-      <c r="D3" s="23" t="s">
+      <c r="D3" s="22" t="s">
         <v>141</v>
       </c>
       <c r="E3" s="14" t="s">
         <v>166</v>
       </c>
-      <c r="F3" s="23" t="s">
+      <c r="F3" s="22" t="s">
         <v>117</v>
       </c>
-      <c r="G3" s="23" t="s">
-        <v>176</v>
-      </c>
-      <c r="H3" s="23" t="s">
+      <c r="G3" s="22" t="s">
+        <v>175</v>
+      </c>
+      <c r="H3" s="22" t="s">
         <v>141</v>
       </c>
       <c r="I3" s="14" t="s">
         <v>166</v>
       </c>
       <c r="J3" s="14" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="K3" s="0" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="136.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="B4" s="23" t="s">
+      <c r="B4" s="22" t="s">
         <v>117</v>
       </c>
-      <c r="C4" s="23" t="s">
+      <c r="C4" s="22" t="s">
         <v>165</v>
       </c>
-      <c r="D4" s="23" t="s">
+      <c r="D4" s="22" t="s">
         <v>141</v>
       </c>
       <c r="E4" s="14" t="s">
         <v>167</v>
       </c>
-      <c r="F4" s="23" t="s">
+      <c r="F4" s="22" t="s">
         <v>117</v>
       </c>
-      <c r="G4" s="23" t="s">
-        <v>176</v>
-      </c>
-      <c r="H4" s="23" t="s">
+      <c r="G4" s="22" t="s">
+        <v>175</v>
+      </c>
+      <c r="H4" s="22" t="s">
         <v>141</v>
       </c>
       <c r="I4" s="14" t="s">
         <v>167</v>
       </c>
       <c r="J4" s="14" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="K4" s="0" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="95.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="B5" s="23" t="s">
+      <c r="B5" s="22" t="s">
         <v>117</v>
       </c>
-      <c r="C5" s="23" t="s">
+      <c r="C5" s="22" t="s">
         <v>165</v>
       </c>
       <c r="D5" s="14"/>
       <c r="E5" s="14"/>
-      <c r="F5" s="23" t="s">
+      <c r="F5" s="22" t="s">
         <v>117</v>
       </c>
-      <c r="G5" s="23" t="s">
-        <v>176</v>
+      <c r="G5" s="22" t="s">
+        <v>175</v>
       </c>
       <c r="H5" s="14"/>
       <c r="I5" s="14"/>
       <c r="J5" s="14" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="K5" s="0" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="95.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3282,25 +3277,25 @@
       <c r="C6" s="14" t="s">
         <v>162</v>
       </c>
-      <c r="D6" s="23" t="s">
+      <c r="D6" s="22" t="s">
         <v>159</v>
       </c>
-      <c r="E6" s="23" t="s">
+      <c r="E6" s="22" t="s">
         <v>164</v>
       </c>
       <c r="F6" s="14" t="s">
         <v>131</v>
       </c>
-      <c r="G6" s="23" t="s">
+      <c r="G6" s="22" t="s">
         <v>132</v>
       </c>
-      <c r="H6" s="23"/>
-      <c r="I6" s="23"/>
+      <c r="H6" s="22"/>
+      <c r="I6" s="22"/>
       <c r="J6" s="14" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="K6" s="0" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
     </row>
   </sheetData>
@@ -3327,7 +3322,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.62222222222222"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="9.21111111111111"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3376,7 +3371,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.62222222222222"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="9.21111111111111"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3390,10 +3385,10 @@
         <v>136</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="F1" s="5" t="s">
         <v>137</v>
@@ -3446,7 +3441,7 @@
         <v>7</v>
       </c>
       <c r="H3" s="10" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="105" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3546,7 +3541,7 @@
         <v>131</v>
       </c>
       <c r="H7" s="10" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="105" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3624,7 +3619,7 @@
         <v>131</v>
       </c>
       <c r="H10" s="10" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
     </row>
   </sheetData>
@@ -3651,7 +3646,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.62222222222222"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="9.21111111111111"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3672,31 +3667,31 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="24" t="s">
+      <c r="A2" s="23" t="s">
         <v>68</v>
       </c>
       <c r="B2" s="8" t="s">
         <v>141</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="D2" s="0" t="s">
         <v>143</v>
       </c>
-      <c r="E2" s="25" t="s">
+      <c r="E2" s="24" t="s">
         <v>131</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="24" t="s">
+      <c r="A3" s="23" t="s">
         <v>69</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>141</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="D3" s="7" t="s">
         <v>131</v>
@@ -3706,14 +3701,14 @@
       </c>
     </row>
     <row r="4" customFormat="false" ht="75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="24" t="s">
+      <c r="A4" s="23" t="s">
         <v>70</v>
       </c>
       <c r="B4" s="8" t="s">
         <v>141</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="D4" s="8" t="s">
         <v>130</v>
@@ -3730,7 +3725,7 @@
         <v>141</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -3760,9 +3755,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.2444444444444"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="19.3037037037037"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.62222222222222"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="23.7148148148148"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="20.7740740740741"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="9.21111111111111"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3822,7 +3817,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.62222222222222"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="9.21111111111111"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3907,7 +3902,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.62222222222222"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="9.21111111111111"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4227,14 +4222,14 @@
   </sheetPr>
   <dimension ref="A1:E65536"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C11" activeCellId="0" sqref="C11"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F4" activeCellId="0" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="40.4444444444444"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="8.62222222222222"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="43.3148148148148"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="9.21111111111111"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4254,7 +4249,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="14" t="s">
         <v>8</v>
       </c>
@@ -4403,7 +4398,7 @@
         <v>155</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>168</v>
+        <v>156</v>
       </c>
       <c r="D11" s="10"/>
       <c r="E11" s="10"/>
@@ -4442,13 +4437,13 @@
   </sheetPr>
   <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="F4" activeCellId="0" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.62222222222222"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="9.21111111111111"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4462,7 +4457,7 @@
         <v>116</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="90" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4476,7 +4471,7 @@
         <v>142</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="105" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4490,7 +4485,7 @@
         <v>142</v>
       </c>
       <c r="D3" s="10" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="105" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4504,7 +4499,7 @@
         <v>167</v>
       </c>
       <c r="D4" s="10" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="120" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4518,7 +4513,7 @@
         <v>167</v>
       </c>
       <c r="D5" s="10" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="105" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4532,7 +4527,7 @@
         <v>130</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="105" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4546,7 +4541,7 @@
         <v>130</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="120" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4560,7 +4555,7 @@
         <v>132</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="120" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4574,7 +4569,7 @@
         <v>132</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
   </sheetData>
@@ -4601,13 +4596,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="59.1037037037037"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.7259259259259"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="11.8962962962963"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15.2296296296296"/>
-    <col collapsed="false" hidden="false" max="9" min="5" style="0" width="11.8962962962963"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="11.5962962962963"/>
-    <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="8.62222222222222"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="63.6962962962963"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.7777777777778"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.5444444444444"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="16.3666666666667"/>
+    <col collapsed="false" hidden="false" max="9" min="5" style="0" width="12.5444444444444"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="12.3481481481481"/>
+    <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="9.21111111111111"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4621,10 +4616,10 @@
         <v>122</v>
       </c>
       <c r="D1" s="5" t="s">
+        <v>171</v>
+      </c>
+      <c r="E1" s="5" t="s">
         <v>172</v>
-      </c>
-      <c r="E1" s="5" t="s">
-        <v>173</v>
       </c>
       <c r="F1" s="5" t="s">
         <v>123</v>
@@ -4633,10 +4628,10 @@
         <v>124</v>
       </c>
       <c r="H1" s="5" t="s">
+        <v>173</v>
+      </c>
+      <c r="I1" s="5" t="s">
         <v>174</v>
-      </c>
-      <c r="I1" s="5" t="s">
-        <v>175</v>
       </c>
       <c r="J1" s="5" t="s">
         <v>139</v>
@@ -4662,7 +4657,7 @@
         <v>117</v>
       </c>
       <c r="G2" s="10" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="H2" s="10" t="s">
         <v>141</v>
@@ -4671,7 +4666,7 @@
         <v>142</v>
       </c>
       <c r="J2" s="10" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4690,12 +4685,12 @@
         <v>117</v>
       </c>
       <c r="G3" s="10" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="H3" s="10"/>
       <c r="I3" s="10"/>
       <c r="J3" s="10" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4709,10 +4704,10 @@
         <v>142</v>
       </c>
       <c r="D4" s="10" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E4" s="10" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F4" s="9" t="s">
         <v>130</v>
@@ -4723,7 +4718,7 @@
       <c r="H4" s="9"/>
       <c r="I4" s="9"/>
       <c r="J4" s="10" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4751,7 +4746,7 @@
       <c r="H5" s="10"/>
       <c r="I5" s="3"/>
       <c r="J5" s="10" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
   </sheetData>
@@ -4770,28 +4765,28 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:K5"/>
+  <dimension ref="A1:M5"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C40" activeCellId="0" sqref="C40"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G14" activeCellId="0" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="54.3296296296296"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.2555555555556"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="18.6888888888889"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.0407407407407"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="11.562962962963"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="17.2148148148148"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="20.5703703703704"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="12.6407407407407"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="12.1"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="11.9666666666667"/>
-    <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="8.36296296296296"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="58.5037037037037"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.2888888888889"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="19.9925925925926"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.9148148148148"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="12.3481481481481"/>
+    <col collapsed="false" hidden="false" max="8" min="6" style="0" width="18.4222222222222"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="22.1481481481481"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="13.4259259259259"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="12.7407407407407"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="12.6407407407407"/>
+    <col collapsed="false" hidden="false" max="1025" min="13" style="0" width="8.81851851851852"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -4802,27 +4797,33 @@
         <v>122</v>
       </c>
       <c r="D1" s="5" t="s">
+        <v>171</v>
+      </c>
+      <c r="E1" s="5" t="s">
         <v>172</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="F1" s="5" t="s">
+        <v>178</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>179</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="J1" s="5" t="s">
         <v>173</v>
       </c>
-      <c r="F1" s="5" t="s">
-        <v>123</v>
-      </c>
-      <c r="G1" s="5" t="s">
-        <v>124</v>
-      </c>
-      <c r="H1" s="5" t="s">
+      <c r="K1" s="5" t="s">
         <v>174</v>
       </c>
-      <c r="I1" s="5" t="s">
-        <v>175</v>
-      </c>
-      <c r="J1" s="5" t="s">
-        <v>179</v>
-      </c>
-      <c r="K1" s="5" t="s">
+      <c r="L1" s="5" t="s">
+        <v>180</v>
+      </c>
+      <c r="M1" s="5" t="s">
         <v>139</v>
       </c>
     </row>
@@ -4834,23 +4835,29 @@
         <v>155</v>
       </c>
       <c r="C2" s="15" t="s">
-        <v>168</v>
-      </c>
-      <c r="D2" s="16"/>
-      <c r="E2" s="15"/>
-      <c r="F2" s="17" t="s">
+        <v>156</v>
+      </c>
+      <c r="D2" s="17" t="s">
         <v>157</v>
       </c>
-      <c r="G2" s="17" t="s">
-        <v>180</v>
-      </c>
-      <c r="H2" s="17"/>
-      <c r="I2" s="17"/>
-      <c r="J2" s="17" t="s">
+      <c r="E2" s="17" t="s">
         <v>181</v>
       </c>
-      <c r="K2" s="17" t="s">
+      <c r="F2" s="15"/>
+      <c r="G2" s="15"/>
+      <c r="H2" s="17" t="s">
+        <v>157</v>
+      </c>
+      <c r="I2" s="17" t="s">
+        <v>181</v>
+      </c>
+      <c r="J2" s="17"/>
+      <c r="K2" s="17"/>
+      <c r="L2" s="17" t="s">
         <v>182</v>
+      </c>
+      <c r="M2" s="17" t="s">
+        <v>183</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4865,19 +4872,21 @@
       </c>
       <c r="D3" s="16"/>
       <c r="E3" s="16"/>
-      <c r="F3" s="17" t="s">
+      <c r="F3" s="16"/>
+      <c r="G3" s="16"/>
+      <c r="H3" s="17" t="s">
         <v>157</v>
       </c>
-      <c r="G3" s="17" t="s">
-        <v>180</v>
-      </c>
-      <c r="H3" s="17"/>
-      <c r="I3" s="17"/>
-      <c r="J3" s="17" t="s">
+      <c r="I3" s="17" t="s">
         <v>181</v>
       </c>
-      <c r="K3" s="17" t="s">
+      <c r="J3" s="17"/>
+      <c r="K3" s="17"/>
+      <c r="L3" s="17" t="s">
         <v>182</v>
+      </c>
+      <c r="M3" s="17" t="s">
+        <v>183</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4888,7 +4897,7 @@
         <v>155</v>
       </c>
       <c r="C4" s="15" t="s">
-        <v>168</v>
+        <v>156</v>
       </c>
       <c r="D4" s="16" t="s">
         <v>141</v>
@@ -4896,23 +4905,29 @@
       <c r="E4" s="16" t="s">
         <v>142</v>
       </c>
-      <c r="F4" s="18" t="s">
+      <c r="F4" s="17" t="s">
         <v>157</v>
       </c>
       <c r="G4" s="17" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="H4" s="18" t="s">
-        <v>141</v>
-      </c>
-      <c r="I4" s="18" t="s">
+        <v>157</v>
+      </c>
+      <c r="I4" s="17" t="s">
+        <v>181</v>
+      </c>
+      <c r="J4" s="18" t="s">
+        <v>141</v>
+      </c>
+      <c r="K4" s="18" t="s">
         <v>142</v>
       </c>
-      <c r="J4" s="18" t="s">
-        <v>181</v>
-      </c>
-      <c r="K4" s="17" t="s">
+      <c r="L4" s="18" t="s">
         <v>182</v>
+      </c>
+      <c r="M4" s="17" t="s">
+        <v>183</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4931,23 +4946,25 @@
       <c r="E5" s="17" t="s">
         <v>142</v>
       </c>
-      <c r="F5" s="17" t="s">
+      <c r="F5" s="17"/>
+      <c r="G5" s="17"/>
+      <c r="H5" s="17" t="s">
         <v>157</v>
       </c>
-      <c r="G5" s="17" t="s">
-        <v>180</v>
-      </c>
-      <c r="H5" s="17" t="s">
-        <v>141</v>
-      </c>
       <c r="I5" s="17" t="s">
+        <v>181</v>
+      </c>
+      <c r="J5" s="17" t="s">
+        <v>141</v>
+      </c>
+      <c r="K5" s="17" t="s">
         <v>142</v>
       </c>
-      <c r="J5" s="17" t="s">
-        <v>181</v>
-      </c>
-      <c r="K5" s="17" t="s">
+      <c r="L5" s="17" t="s">
         <v>182</v>
+      </c>
+      <c r="M5" s="17" t="s">
+        <v>183</v>
       </c>
     </row>
   </sheetData>
@@ -4974,9 +4991,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="50.7333333333333"/>
-    <col collapsed="false" hidden="false" max="9" min="2" style="0" width="9.27777777777778"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="8.62222222222222"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="54.5814814814815"/>
+    <col collapsed="false" hidden="false" max="9" min="2" style="0" width="9.8962962962963"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="9.21111111111111"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4990,10 +5007,10 @@
         <v>122</v>
       </c>
       <c r="D1" s="5" t="s">
+        <v>171</v>
+      </c>
+      <c r="E1" s="5" t="s">
         <v>172</v>
-      </c>
-      <c r="E1" s="5" t="s">
-        <v>173</v>
       </c>
       <c r="F1" s="5" t="s">
         <v>123</v>
@@ -5002,10 +5019,10 @@
         <v>124</v>
       </c>
       <c r="H1" s="5" t="s">
+        <v>173</v>
+      </c>
+      <c r="I1" s="5" t="s">
         <v>174</v>
-      </c>
-      <c r="I1" s="5" t="s">
-        <v>175</v>
       </c>
       <c r="J1" s="5" t="s">
         <v>139</v>
@@ -5022,10 +5039,10 @@
         <v>142</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F2" s="9" t="s">
         <v>128</v>
@@ -5036,7 +5053,7 @@
       <c r="H2" s="9"/>
       <c r="I2" s="9"/>
       <c r="J2" s="10" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5050,10 +5067,10 @@
         <v>142</v>
       </c>
       <c r="D3" s="10" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E3" s="10" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F3" s="10" t="s">
         <v>141</v>
@@ -5068,7 +5085,7 @@
         <v>130</v>
       </c>
       <c r="J3" s="10" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
     </row>
   </sheetData>

</xml_diff>